<commit_message>
Add tests and allure-results
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="100">
   <si>
     <t>Страница авторизации</t>
   </si>
@@ -203,24 +203,6 @@
     <t>Пользователь авторизован, находится на странице "News"</t>
   </si>
   <si>
-    <t>Развернуть новость</t>
-  </si>
-  <si>
-    <t>1. Нажать на галочку в правой части новости</t>
-  </si>
-  <si>
-    <t>Новость разворачивается</t>
-  </si>
-  <si>
-    <t>1. Нажать на кнопку "Фильтр" (находится перед плюсиком в кружке)</t>
-  </si>
-  <si>
-    <t>Открылась страница "Filter news"</t>
-  </si>
-  <si>
-    <t>Открытие фильтрация новостей</t>
-  </si>
-  <si>
     <t>Фильтрация новостей по категории "Объявление"</t>
   </si>
   <si>
@@ -296,66 +278,9 @@
 4. Нажать на кнопку "Filter"</t>
   </si>
   <si>
-    <t>Фильтрация новостей с вводом только конечного значения периода</t>
-  </si>
-  <si>
-    <t>Фильтрация новостей с вводом только начального значения периода</t>
-  </si>
-  <si>
-    <t>Фильтрация новостей за период</t>
-  </si>
-  <si>
-    <t>1. Нажать на кнопку "Фильтр" (находится перед плюсиком в кружке)
-2. Нажать на левую строку "DD.MM.YYYY"
-3. Выбрать любую дату
-4. Нажать на кнопку "Filter"</t>
-  </si>
-  <si>
-    <t>1. Нажать на кнопку "Фильтр" (находится перед плюсиком в кружке)
-2. Нажать на левую строку "DD.MM.YYYY"
-3. Выбрать любую дату
-4. Нажать на правую строку "DD.MM.YYYY"
-5. Выбрать любую дату
-6. Нажать на кнопку "Filter"</t>
-  </si>
-  <si>
-    <t>1. Нажать на кнопку "Фильтр" (находится перед плюсиком в кружке)
-2. Нажать на правую строку "DD.MM.YYYY"
-3. Выбрать любую дату
-4. Нажать на кнопку "Filter"</t>
-  </si>
-  <si>
-    <t>Вывод сообщения "Wrong period"</t>
-  </si>
-  <si>
-    <t>Выводятся отфильтрованные новости за заданный период</t>
-  </si>
-  <si>
     <t>Новая претензия появилась в "Claims"</t>
   </si>
   <si>
-    <t>Отмена фильтрации новостей</t>
-  </si>
-  <si>
-    <t>1. Нажать на кнопку "Фильтр" (находится перед плюсиком в кружке)
-2. Нажать на кнопку "Cancel"</t>
-  </si>
-  <si>
-    <t>Страница тематических цитат</t>
-  </si>
-  <si>
-    <t>Пользователь авторизован, находится на странице "News", "Clains" или "Main"</t>
-  </si>
-  <si>
-    <t>1. Нажать на иконку бабочки в верхней части экрана</t>
-  </si>
-  <si>
-    <t>Открылась страница тематических цитат</t>
-  </si>
-  <si>
-    <t>Открылась страница "News", фильтрация не применилась</t>
-  </si>
-  <si>
     <t>Открылась страница с сообщениями категории "Нужна помощь"</t>
   </si>
   <si>
@@ -389,20 +314,7 @@
     <t>Пользователь авторизован, переход на страницу "Main"</t>
   </si>
   <si>
-    <t>Переход на страницу тематических цитат</t>
-  </si>
-  <si>
     <t>Low</t>
-  </si>
-  <si>
-    <t>Развернуть тематическую цитату</t>
-  </si>
-  <si>
-    <t>1. Нажать на иконку бабочки в верхней части экрана
-2. Нажать на галочку возле любой цитаты</t>
-  </si>
-  <si>
-    <t>Цитата развернулась</t>
   </si>
   <si>
     <t>Покрытие автотестами</t>
@@ -453,6 +365,36 @@
     <t>1. Запустить приложение
 2.  Ввести в поле "password" значение password2
 3. Нажать кнопку "Sign in"</t>
+  </si>
+  <si>
+    <t>Страница "About"</t>
+  </si>
+  <si>
+    <t>Переход по ссылке "Политика конфиденциальности"</t>
+  </si>
+  <si>
+    <t>Переход по ссылке "Пользовательское соглашение"</t>
+  </si>
+  <si>
+    <t>Пользователь авторизован, находится на странице"About"</t>
+  </si>
+  <si>
+    <t>1. Нажать на ссылку под "Privacy Policy"</t>
+  </si>
+  <si>
+    <t>1. Нажать на ссылку под "Terms of use"</t>
+  </si>
+  <si>
+    <t>Переход по ссылке</t>
+  </si>
+  <si>
+    <t>Сортировка новостей</t>
+  </si>
+  <si>
+    <t>1. Нажать на кнопку "Сортировка" (две разнонаправленные вертикальные стрелки)</t>
+  </si>
+  <si>
+    <t>Новости отсортировались</t>
   </si>
 </sst>
 </file>
@@ -498,7 +440,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -540,6 +482,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -570,7 +518,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -602,17 +550,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -888,7 +842,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -896,11 +850,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,43 +869,43 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>102</v>
+        <v>82</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -961,20 +915,20 @@
         <v>3</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>103</v>
+        <v>75</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -984,20 +938,20 @@
         <v>4</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="14" t="s">
-        <v>103</v>
+      <c r="G4" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1007,20 +961,20 @@
         <v>8</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="14" t="s">
-        <v>103</v>
+      <c r="G5" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -1030,20 +984,20 @@
         <v>11</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="14" t="s">
-        <v>103</v>
+      <c r="G6" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1053,31 +1007,31 @@
         <v>13</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="14" t="s">
-        <v>103</v>
+      <c r="G7" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>6</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1090,17 +1044,17 @@
         <v>18</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>103</v>
+        <v>72</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>7</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -1113,17 +1067,17 @@
         <v>19</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>103</v>
+        <v>73</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>8</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1136,17 +1090,17 @@
         <v>20</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>103</v>
+        <v>74</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>9</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -1159,17 +1113,17 @@
         <v>23</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>103</v>
+        <v>73</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>10</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="14" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -1182,28 +1136,28 @@
         <v>24</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>103</v>
+        <v>72</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
     </row>
     <row r="15" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>11</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -1216,17 +1170,17 @@
         <v>33</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>103</v>
+        <v>64</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>12</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="14" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -1241,15 +1195,15 @@
       <c r="F16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="14" t="s">
-        <v>103</v>
+      <c r="G16" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>13</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="14" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="9" t="s">
@@ -1264,15 +1218,15 @@
       <c r="F17" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="14" t="s">
-        <v>103</v>
+      <c r="G17" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>14</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="14" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="9" t="s">
@@ -1287,15 +1241,15 @@
       <c r="F18" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="14" t="s">
-        <v>103</v>
+      <c r="G18" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>15</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="14" t="s">
         <v>39</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -1310,15 +1264,15 @@
       <c r="F19" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="14" t="s">
-        <v>103</v>
+      <c r="G19" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>16</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="14" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -1333,15 +1287,15 @@
       <c r="F20" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="14" t="s">
-        <v>103</v>
+      <c r="G20" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>17</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="14" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -1356,50 +1310,50 @@
       <c r="F21" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="14" t="s">
-        <v>103</v>
+      <c r="G21" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+    </row>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>18</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>47</v>
+      <c r="B23" s="14" t="s">
+        <v>97</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>46</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>19</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>52</v>
+      <c r="B24" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>17</v>
@@ -1408,21 +1362,21 @@
         <v>46</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>103</v>
+        <v>71</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>20</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>53</v>
+      <c r="B25" s="14" t="s">
+        <v>49</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>17</v>
@@ -1431,21 +1385,21 @@
         <v>46</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>103</v>
+        <v>70</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>21</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>55</v>
+      <c r="B26" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>17</v>
@@ -1454,21 +1408,21 @@
         <v>46</v>
       </c>
       <c r="E26" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F26" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>103</v>
+      <c r="G26" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>22</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>56</v>
+      <c r="B27" s="14" t="s">
+        <v>51</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>17</v>
@@ -1477,21 +1431,21 @@
         <v>46</v>
       </c>
       <c r="E27" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F27" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>103</v>
+      <c r="G27" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>23</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>57</v>
+      <c r="B28" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>17</v>
@@ -1500,21 +1454,21 @@
         <v>46</v>
       </c>
       <c r="E28" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>103</v>
+      <c r="G28" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>24</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>58</v>
+      <c r="B29" s="14" t="s">
+        <v>53</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>17</v>
@@ -1523,21 +1477,21 @@
         <v>46</v>
       </c>
       <c r="E29" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F29" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>103</v>
+      <c r="G29" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>25</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>59</v>
+      <c r="B30" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>17</v>
@@ -1546,21 +1500,21 @@
         <v>46</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>103</v>
+        <v>58</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>26</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>60</v>
+      <c r="B31" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>17</v>
@@ -1569,185 +1523,70 @@
         <v>46</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+        <v>65</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
         <v>27</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+      <c r="B33" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
         <v>28</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
-        <v>29</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>70</v>
+      <c r="B34" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>75</v>
+        <v>93</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
-        <v>30</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
-        <v>31</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-    </row>
-    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
-        <v>32</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
-        <v>33</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>103</v>
+        <v>96</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1756,7 +1595,7 @@
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A32:G32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>